<commit_message>
Cambios menores,se renombro manto_feeder por mantto_feeder
</commit_message>
<xml_diff>
--- a/MF-64_23760055.xlsx
+++ b/MF-64_23760055.xlsx
@@ -2,23 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11385" windowWidth="21600" xWindow="0" yWindow="3285"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="m/d/yyyy;@" numFmtId="164"/>
-    <numFmt formatCode="m/d/yy;@" numFmtId="165"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -53,18 +51,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
@@ -429,18 +424,17 @@
   </sheetPr>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="5" width="20"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="5" width="13"/>
-    <col bestFit="1" customWidth="1" max="14" min="11" style="5" width="9.7109375"/>
+    <col customWidth="1" max="1" min="1" width="20"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="13"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26.25" r="1" s="5">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Nombre</t>
@@ -451,7 +445,7 @@
           <t>Apellido</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>datos fusionados</t>
         </is>
@@ -562,77 +556,55 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>p</t>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>
     <row r="4"/>
-    <row r="5">
-      <c r="J5" s="3" t="n">
-        <v>45086</v>
-      </c>
-      <c r="K5" s="3" t="n">
-        <v>45087</v>
-      </c>
-      <c r="L5" s="3" t="n">
-        <v>45088</v>
-      </c>
-      <c r="M5" s="3" t="n">
-        <v>45089</v>
-      </c>
-      <c r="N5" s="3" t="n">
-        <v>45090</v>
-      </c>
-      <c r="O5" s="3" t="n">
-        <v>45091</v>
-      </c>
-      <c r="P5" s="3" t="n">
-        <v>45092</v>
-      </c>
-      <c r="Q5" s="3" t="n">
-        <v>45093</v>
-      </c>
-      <c r="R5" s="3" t="n">
-        <v>45094</v>
-      </c>
-      <c r="S5" s="3" t="n">
-        <v>45095</v>
-      </c>
-      <c r="T5" s="3" t="n">
-        <v>45096</v>
-      </c>
-      <c r="U5" s="3" t="n">
-        <v>45097</v>
-      </c>
-      <c r="V5" s="3" t="n">
-        <v>45098</v>
-      </c>
-      <c r="W5" s="3" t="n">
-        <v>45099</v>
-      </c>
-      <c r="X5" s="3" t="n">
-        <v>45100</v>
-      </c>
-      <c r="Y5" s="3" t="n">
-        <v>45101</v>
-      </c>
-      <c r="Z5" s="3" t="n">
-        <v>45102</v>
+    <row r="5"/>
+    <row r="6">
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>23760055</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n"/>
-    </row>
+    <row r="7"/>
     <row r="8"/>
     <row r="9"/>
     <row r="10"/>
@@ -649,14 +621,5 @@
     <mergeCell ref="A10:F17"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup orientation="portrait" verticalDpi="0"/>
-  <headerFooter>
-    <oddHeader/>
-    <oddFooter>&amp;C&amp;"Calibri"&amp;10 &amp;K0000FF_x000d_# This data is internal to Brunswick._x000d_&amp;1#&amp;"Calibri"&amp;10 &amp;K0000FF This data is internal to Brunswick.</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>